<commit_message>
kat, opis, większe wyświetlanie
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="930" windowWidth="25140" windowHeight="16350" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,12 +45,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -399,15 +396,15 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="9.140625" customWidth="1" style="1" min="1" max="1"/>
     <col width="10.140625" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
-    <col width="9.140625" customWidth="1" style="1" min="3" max="3"/>
-    <col width="9.140625" customWidth="1" style="1" min="4" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="3" max="5"/>
+    <col width="9.140625" customWidth="1" style="1" min="6" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -437,6 +434,16 @@
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>Data</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>Kategoria</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>Opis</t>
         </is>
       </c>
     </row>

</xml_diff>